<commit_message>
Finish random suggestion (without GPA)
</commit_message>
<xml_diff>
--- a/Src/test.xlsx
+++ b/Src/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qiaom\source\repos\SDWIII\Eagle\Src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C171EE-0729-4F44-A456-43370203B06A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32347349-3A9E-410E-96D6-A8D2C8393A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2088" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,102 @@
   </si>
   <si>
     <t>135@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jason</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coco</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rose</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tony</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jessica</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jeremy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n789</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n135</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l123135</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l712389</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l45426</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l12323</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l12323@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l45426@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l712389@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l123135@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m123@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m456@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n789@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n135@qq.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -408,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -461,7 +557,7 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -475,7 +571,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>3.3</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -489,7 +585,119 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>3.7</v>
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9">
+        <v>3.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13">
+        <v>3.08</v>
       </c>
     </row>
   </sheetData>
@@ -499,8 +707,16 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{0A3620FB-41B3-4359-B8E6-CD5E823B92ED}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{1D12840E-645D-49B3-8B91-FEDCEFBDADF3}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{026DE335-0030-49C4-8D86-79D5C52EB79B}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{642FBF87-68A6-4252-AB62-3F1C7C24F800}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{F939FF8F-DEA4-4C06-AE8F-7DDB722AB2C0}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{4009D2B4-3BCE-4A27-BFCF-99468ABF3F72}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{84E9DD2C-09FF-41DC-9418-E845E5828106}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{424AB54A-B89A-45DB-BA46-715A6AD72A3C}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{2D8B9602-CB36-4141-83BB-34520A862798}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{D4CC9954-6CD5-4B2D-92A6-E446C055AD22}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{9D50740F-3FAB-4823-B362-CB653AFA9702}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change the generate student
</commit_message>
<xml_diff>
--- a/Src/test.xlsx
+++ b/Src/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qiaom\source\repos\SDWIII\Eagle\Src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32347349-3A9E-410E-96D6-A8D2C8393A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71ABE9A-9B89-4F1A-BBDF-D6E95328B478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2088" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2124" yWindow="2208" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,10 +59,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>123@qq.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>456@qq.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -168,6 +164,10 @@
   </si>
   <si>
     <t>n135@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>129@qq.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -507,7 +507,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -537,10 +537,10 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -554,7 +554,7 @@
         <v>456</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>3.97</v>
@@ -568,7 +568,7 @@
         <v>789</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>3.23</v>
@@ -582,7 +582,7 @@
         <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>3.55</v>
@@ -590,13 +590,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D6">
         <v>2.89</v>
@@ -604,13 +604,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>2.64</v>
@@ -618,13 +618,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>3.31</v>
@@ -632,13 +632,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>3.19</v>
@@ -646,13 +646,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>3.6</v>
@@ -660,13 +660,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>3.36</v>
@@ -674,13 +674,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>3.57</v>
@@ -688,13 +688,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>3.08</v>

</xml_diff>

<commit_message>
Update part of the forming method 4
</commit_message>
<xml_diff>
--- a/Src/test.xlsx
+++ b/Src/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qiaom\source\repos\SDWIII\Eagle\Src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC21EC90-A8FC-48AD-8254-E3F39C1BCDDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F4D728-C37E-4EBB-8BFB-65D7C6237295}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2124" yWindow="2208" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,38 +107,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>l123135</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l712389</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l45426</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l12323</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l12323@qq.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l45426@qq.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l712389@qq.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l123135@qq.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>m123@qq.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,15 +147,95 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>oooo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ll123</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ll123@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jelie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rumer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ll456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ll456@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ll789</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ll789@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Naomy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ll135</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ll135@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l789</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l135</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l123@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l456@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l789@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l135@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Otis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ll357</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ll357@qq.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -524,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -557,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -574,7 +622,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>3.97</v>
@@ -585,10 +633,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>3.23</v>
@@ -599,10 +647,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>3.55</v>
@@ -613,10 +661,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>2.89</v>
@@ -627,10 +675,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>2.64</v>
@@ -641,10 +689,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>3.31</v>
@@ -655,10 +703,10 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>3.19</v>
@@ -672,7 +720,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>3.6</v>
@@ -686,7 +734,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>3.36</v>
@@ -700,7 +748,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>3.57</v>
@@ -714,7 +762,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>3.08</v>
@@ -722,16 +770,72 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D16">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="D14">
-        <v>4</v>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18">
+        <v>3.14</v>
       </c>
     </row>
   </sheetData>
@@ -750,8 +854,12 @@
     <hyperlink ref="C12" r:id="rId11" xr:uid="{D4CC9954-6CD5-4B2D-92A6-E446C055AD22}"/>
     <hyperlink ref="C13" r:id="rId12" xr:uid="{9D50740F-3FAB-4823-B362-CB653AFA9702}"/>
     <hyperlink ref="C14" r:id="rId13" xr:uid="{65A231DD-B760-47E9-B12C-470DB4A1D945}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{46EEE23B-1B7A-43B1-8A2E-7A2B72ACFA6C}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{ED81B31D-B5CF-4B05-8732-115AA6603A7F}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{592EAC8B-4758-4907-A8FD-A6CF80B7B154}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{F720155D-2811-4937-B282-04076C76BEA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix bugs && add is_finished attribute
</commit_message>
<xml_diff>
--- a/Src/test.xlsx
+++ b/Src/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qiaom\source\repos\SDWIII\Eagle\Src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F4D728-C37E-4EBB-8BFB-65D7C6237295}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6F3051-BE65-439A-BA76-8692CF35AFDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -236,6 +236,14 @@
   </si>
   <si>
     <t>ll357@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m579</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m579@qq.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -575,7 +583,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -619,10 +627,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>3.97</v>

</xml_diff>